<commit_message>
change the heavyweight output to be >109; closes #911
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/records/exportRecords.xlsx
+++ b/owlcms/src/main/resources/templates/records/exportRecords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288FD7C1-D42D-4E4F-B195-054D142C4D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E4482B-A5EF-40FE-A4B7-C671422038A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NewRecords" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,94 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jean-François Lamy</author>
+  </authors>
+  <commentList>
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{C6FF4C17-205A-4117-9526-D4356C492D3F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>owlcms:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+for non-heavyweight category use a number
+45 59 55 64 ...
+for heavyweight category use &gt; followed by number
+&gt;81 &gt;87 &gt;102 &gt;109 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{E929A3F5-8334-4A41-8BFE-3F8D0356CC97}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>owlcms:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Columns from K to O are optional and are not used by the system
+You can leave them empty.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{17BBEB5E-9C88-41B3-B3AF-34E640F0734C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">owlcms:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Column P indicates the session in which the record was set.
+This indicates a new record established in the current competition.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
@@ -101,9 +189,6 @@
     <t>${r.bwCatLower}</t>
   </si>
   <si>
-    <t>${r.bwCatUpper}</t>
-  </si>
-  <si>
     <t>${r.recordLift}</t>
   </si>
   <si>
@@ -138,13 +223,16 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>${r.bwCatString}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +263,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -202,7 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -252,16 +353,19 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -587,11 +691,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,9 +706,10 @@
     <col min="4" max="4" width="7.85546875" style="7" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" style="15" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" style="15" customWidth="1"/>
-    <col min="7" max="8" width="8.5703125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="20" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" style="7" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="20" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="20" customWidth="1"/>
     <col min="11" max="11" width="33.140625" style="7" customWidth="1"/>
     <col min="12" max="12" width="11" style="13" customWidth="1"/>
     <col min="13" max="13" width="10.5703125" style="7" customWidth="1"/>
@@ -631,13 +736,13 @@
         <v>11</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="16" t="s">
-        <v>30</v>
+      <c r="H1" s="21" t="s">
+        <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>0</v>
@@ -675,7 +780,7 @@
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="H2" s="18"/>
       <c r="I2" s="9"/>
       <c r="J2" s="18"/>
       <c r="K2" s="9"/>
@@ -704,32 +809,32 @@
       <c r="G3" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="J3" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="K3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="L3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="M3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="N3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="P3" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>33</v>
       </c>
       <c r="Q3" s="9"/>
     </row>
@@ -743,7 +848,7 @@
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="H4" s="18"/>
       <c r="I4" s="3"/>
       <c r="J4" s="19"/>
       <c r="K4" s="3"/>
@@ -759,7 +864,7 @@
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="H5" s="18"/>
       <c r="I5" s="3"/>
       <c r="J5" s="19"/>
       <c r="K5" s="3"/>
@@ -775,7 +880,7 @@
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="H6" s="18"/>
       <c r="I6" s="3"/>
       <c r="J6" s="19"/>
       <c r="K6" s="3"/>
@@ -791,7 +896,7 @@
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="H7" s="18"/>
       <c r="I7" s="3"/>
       <c r="J7" s="19"/>
       <c r="K7" s="3"/>
@@ -807,7 +912,7 @@
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="H8" s="18"/>
       <c r="I8" s="3"/>
       <c r="J8" s="19"/>
       <c r="K8" s="3"/>
@@ -823,7 +928,7 @@
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
+      <c r="H9" s="18"/>
       <c r="I9" s="3"/>
       <c r="J9" s="19"/>
       <c r="K9" s="3"/>
@@ -839,7 +944,7 @@
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="H10" s="18"/>
       <c r="I10" s="3"/>
       <c r="J10" s="19"/>
       <c r="K10" s="3"/>
@@ -855,7 +960,7 @@
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="H11" s="18"/>
       <c r="I11" s="3"/>
       <c r="J11" s="19"/>
       <c r="K11" s="3"/>
@@ -871,7 +976,7 @@
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="H12" s="18"/>
       <c r="I12" s="3"/>
       <c r="J12" s="19"/>
       <c r="K12" s="3"/>
@@ -887,7 +992,7 @@
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="H13" s="18"/>
       <c r="I13" s="3"/>
       <c r="J13" s="19"/>
       <c r="K13" s="3"/>
@@ -903,7 +1008,7 @@
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="H14" s="18"/>
       <c r="I14" s="3"/>
       <c r="J14" s="19"/>
       <c r="K14" s="3"/>
@@ -919,7 +1024,7 @@
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+      <c r="H15" s="18"/>
       <c r="I15" s="3"/>
       <c r="J15" s="19"/>
       <c r="K15" s="3"/>
@@ -935,7 +1040,7 @@
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
+      <c r="H16" s="18"/>
       <c r="I16" s="3"/>
       <c r="J16" s="19"/>
       <c r="K16" s="3"/>
@@ -951,7 +1056,7 @@
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="H17" s="18"/>
       <c r="I17" s="3"/>
       <c r="J17" s="19"/>
       <c r="K17" s="3"/>
@@ -967,7 +1072,7 @@
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="H18" s="18"/>
       <c r="I18" s="3"/>
       <c r="J18" s="19"/>
       <c r="K18" s="3"/>
@@ -983,7 +1088,7 @@
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="3"/>
       <c r="J19" s="19"/>
       <c r="K19" s="3"/>
@@ -999,7 +1104,7 @@
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
+      <c r="H20" s="18"/>
       <c r="I20" s="3"/>
       <c r="J20" s="19"/>
       <c r="K20" s="3"/>
@@ -1015,7 +1120,7 @@
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
+      <c r="H21" s="18"/>
       <c r="I21" s="3"/>
       <c r="J21" s="19"/>
       <c r="K21" s="3"/>
@@ -1031,7 +1136,7 @@
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
+      <c r="H22" s="18"/>
       <c r="I22" s="3"/>
       <c r="J22" s="19"/>
       <c r="K22" s="3"/>
@@ -1047,7 +1152,7 @@
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
+      <c r="H23" s="18"/>
       <c r="I23" s="3"/>
       <c r="J23" s="19"/>
       <c r="K23" s="3"/>
@@ -1063,7 +1168,7 @@
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
+      <c r="H24" s="18"/>
       <c r="I24" s="3"/>
       <c r="J24" s="19"/>
       <c r="K24" s="3"/>
@@ -1079,7 +1184,7 @@
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
+      <c r="H25" s="18"/>
       <c r="I25" s="3"/>
       <c r="J25" s="19"/>
       <c r="K25" s="3"/>
@@ -1095,7 +1200,7 @@
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
+      <c r="H26" s="18"/>
       <c r="I26" s="3"/>
       <c r="J26" s="19"/>
       <c r="K26" s="3"/>
@@ -1111,7 +1216,7 @@
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
+      <c r="H27" s="18"/>
       <c r="I27" s="3"/>
       <c r="J27" s="19"/>
       <c r="K27" s="3"/>
@@ -1127,7 +1232,7 @@
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
+      <c r="H28" s="18"/>
       <c r="I28" s="3"/>
       <c r="J28" s="19"/>
       <c r="K28" s="3"/>
@@ -1143,7 +1248,7 @@
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
+      <c r="H29" s="18"/>
       <c r="I29" s="3"/>
       <c r="J29" s="19"/>
       <c r="K29" s="3"/>
@@ -1159,7 +1264,7 @@
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
+      <c r="H30" s="18"/>
       <c r="I30" s="3"/>
       <c r="J30" s="19"/>
       <c r="K30" s="3"/>
@@ -1175,7 +1280,7 @@
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
+      <c r="H31" s="18"/>
       <c r="I31" s="3"/>
       <c r="J31" s="19"/>
       <c r="K31" s="3"/>
@@ -1195,7 +1300,7 @@
       <formula1>0</formula1>
       <formula2>120</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:H1048576" xr:uid="{53FB7450-D8BD-4FB4-A0E8-29CC05EF8875}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576 H1:H2 H4:H1048576" xr:uid="{53FB7450-D8BD-4FB4-A0E8-29CC05EF8875}">
       <formula1>0</formula1>
       <formula2>250</formula2>
     </dataValidation>
@@ -1206,6 +1311,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1238,12 +1344,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix for records export/import
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/records/exportRecords.xlsx
+++ b/owlcms/src/main/resources/templates/records/exportRecords.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E4482B-A5EF-40FE-A4B7-C671422038A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B367115-C037-4A1F-95CA-6D3B1ECA6F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NewRecords" sheetId="1" r:id="rId1"/>
-    <sheet name="values" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -118,7 +117,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Lift</t>
   </si>
@@ -150,9 +149,6 @@
     <t>AgeGroup</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
     <t>ageLow</t>
   </si>
   <si>
@@ -219,13 +215,10 @@
     <t>${r.groupNameString}</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>${r.bwCatString}</t>
+  </si>
+  <si>
+    <t>M/F</t>
   </si>
 </sst>
 </file>
@@ -695,7 +688,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,19 +723,19 @@
         <v>9</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="H1" s="21" t="s">
         <v>28</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>0</v>
@@ -766,13 +759,13 @@
         <v>6</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -789,58 +782,58 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="H3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="9" t="s">
+      <c r="J3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="K3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="L3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="M3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="9" t="s">
-        <v>27</v>
-      </c>
       <c r="N3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="P3" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>32</v>
       </c>
       <c r="Q3" s="9"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -1317,42 +1310,12 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DD6A1ACE-E119-406B-B54E-8F08A2EE531D}">
           <x14:formula1>
-            <xm:f>values!$A$2:$A$3</xm:f>
+            <xm:f>#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D4</xm:sqref>
+          <xm:sqref>D2 D4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A7292F-CD7A-44ED-9ECC-F46A88F50B15}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>